<commit_message>
Have gone through a lot of small changes but now added sp. to unknowns so am redoing things because I found wrong things during the final check of species independent list
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_species-list-with-native-status_LO.xlsx
+++ b/data/raw/from-Master_species-list-with-native-status_LO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1702" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F11D1087-B267-47BC-958F-312390040B12}"/>
+  <xr:revisionPtr revIDLastSave="1703" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBCC5B48-11FE-42B6-B92A-A7D98E45CC41}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2866,8 +2866,8 @@
   <dimension ref="A1:D473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A419" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A443" sqref="A443"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A114" sqref="A114:XFD114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4461,7 +4461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>215</v>
       </c>

</xml_diff>

<commit_message>
Made it to 5.1 species.de after adding sp. to capture more location-dependent species
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_species-list-with-native-status_LO.xlsx
+++ b/data/raw/from-Master_species-list-with-native-status_LO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1703" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBCC5B48-11FE-42B6-B92A-A7D98E45CC41}"/>
+  <xr:revisionPtr revIDLastSave="1704" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2DF33F8-985F-4C86-A728-A6032D4B33A3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1679,9 +1679,6 @@
     <t>PROACASPP</t>
   </si>
   <si>
-    <t>Mesquite/Acacia species</t>
-  </si>
-  <si>
     <t>PSCA11</t>
   </si>
   <si>
@@ -2346,6 +2343,9 @@
   </si>
   <si>
     <t xml:space="preserve">Trifolium sp. </t>
+  </si>
+  <si>
+    <t>Mesquite/Acacia spp.</t>
   </si>
 </sst>
 </file>
@@ -2866,8 +2866,8 @@
   <dimension ref="A1:D473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A114" sqref="A114:XFD114"/>
+      <pane ySplit="1" topLeftCell="A333" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B351" sqref="B351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2881,7 +2881,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -3027,7 +3027,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -3097,7 +3097,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -3178,7 +3178,7 @@
         <v>57</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -3195,7 +3195,7 @@
         <v>37</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -3209,7 +3209,7 @@
         <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
@@ -3223,7 +3223,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -3293,7 +3293,7 @@
         <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -3385,10 +3385,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>693</v>
+      </c>
+      <c r="B37" t="s">
         <v>694</v>
-      </c>
-      <c r="B37" t="s">
-        <v>695</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -3475,7 +3475,7 @@
         <v>91</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D43" t="s">
         <v>4</v>
@@ -3570,10 +3570,10 @@
         <v>336</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
@@ -3587,7 +3587,7 @@
         <v>105</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
@@ -3643,7 +3643,7 @@
         <v>113</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D55" t="s">
         <v>4</v>
@@ -3727,7 +3727,7 @@
         <v>125</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D61" t="s">
         <v>4</v>
@@ -3763,10 +3763,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>697</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>698</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
@@ -3861,13 +3861,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>700</v>
-      </c>
       <c r="C71" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D71" t="s">
         <v>4</v>
@@ -3951,7 +3951,7 @@
         <v>152</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D77" t="s">
         <v>4</v>
@@ -4147,7 +4147,7 @@
         <v>178</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D91" t="s">
         <v>4</v>
@@ -4161,7 +4161,7 @@
         <v>180</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D92" t="s">
         <v>4</v>
@@ -4203,7 +4203,7 @@
         <v>186</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D95" t="s">
         <v>4</v>
@@ -4217,7 +4217,7 @@
         <v>188</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D96" t="s">
         <v>4</v>
@@ -4315,7 +4315,7 @@
         <v>202</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D103" t="s">
         <v>4</v>
@@ -4365,10 +4365,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B107" t="s">
         <v>701</v>
-      </c>
-      <c r="B107" t="s">
-        <v>702</v>
       </c>
       <c r="C107" t="s">
         <v>7</v>
@@ -4427,7 +4427,7 @@
         <v>213</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D111" t="s">
         <v>0</v>
@@ -4441,7 +4441,7 @@
         <v>38</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D112" t="s">
         <v>0</v>
@@ -4477,10 +4477,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="B115" t="s">
         <v>694</v>
-      </c>
-      <c r="B115" t="s">
-        <v>695</v>
       </c>
       <c r="C115" t="s">
         <v>7</v>
@@ -4525,7 +4525,7 @@
         <v>105</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D118" t="s">
         <v>0</v>
@@ -4609,7 +4609,7 @@
         <v>232</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D124" t="s">
         <v>0</v>
@@ -4679,7 +4679,7 @@
         <v>241</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D129" t="s">
         <v>0</v>
@@ -4757,10 +4757,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B135" t="s">
         <v>703</v>
-      </c>
-      <c r="B135" t="s">
-        <v>704</v>
       </c>
       <c r="C135" t="s">
         <v>7</v>
@@ -4791,7 +4791,7 @@
         <v>180</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D137" t="s">
         <v>0</v>
@@ -4805,7 +4805,7 @@
         <v>252</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D138" t="s">
         <v>0</v>
@@ -4819,7 +4819,7 @@
         <v>188</v>
       </c>
       <c r="C139" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D139" t="s">
         <v>0</v>
@@ -4855,10 +4855,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B142" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C142" t="s">
         <v>7</v>
@@ -4889,7 +4889,7 @@
         <v>39</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D144" t="s">
         <v>1</v>
@@ -4931,7 +4931,7 @@
         <v>67</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D147" t="s">
         <v>1</v>
@@ -5015,7 +5015,7 @@
         <v>105</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D153" t="s">
         <v>1</v>
@@ -5043,7 +5043,7 @@
         <v>113</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D155" t="s">
         <v>1</v>
@@ -5211,7 +5211,7 @@
         <v>273</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D167" t="s">
         <v>1</v>
@@ -5225,7 +5225,7 @@
         <v>275</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D168" t="s">
         <v>1</v>
@@ -5239,7 +5239,7 @@
         <v>252</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D169" t="s">
         <v>1</v>
@@ -5561,7 +5561,7 @@
         <v>38</v>
       </c>
       <c r="C192" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D192" t="s">
         <v>258</v>
@@ -5603,7 +5603,7 @@
         <v>319</v>
       </c>
       <c r="C195" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D195" t="s">
         <v>258</v>
@@ -5653,10 +5653,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B199" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C199" t="s">
         <v>205</v>
@@ -5799,7 +5799,7 @@
         <v>337</v>
       </c>
       <c r="C209" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D209" t="s">
         <v>258</v>
@@ -5813,7 +5813,7 @@
         <v>105</v>
       </c>
       <c r="C210" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D210" t="s">
         <v>258</v>
@@ -5821,10 +5821,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="B211" t="s">
         <v>708</v>
-      </c>
-      <c r="B211" t="s">
-        <v>709</v>
       </c>
       <c r="C211" t="s">
         <v>7</v>
@@ -5863,10 +5863,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="B214" t="s">
         <v>710</v>
-      </c>
-      <c r="B214" t="s">
-        <v>711</v>
       </c>
       <c r="C214" t="s">
         <v>205</v>
@@ -5911,7 +5911,7 @@
         <v>347</v>
       </c>
       <c r="C217" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D217" t="s">
         <v>258</v>
@@ -6009,7 +6009,7 @@
         <v>360</v>
       </c>
       <c r="C224" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D224" t="s">
         <v>258</v>
@@ -6073,10 +6073,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="B229" t="s">
         <v>712</v>
-      </c>
-      <c r="B229" t="s">
-        <v>713</v>
       </c>
       <c r="C229" t="s">
         <v>205</v>
@@ -6191,7 +6191,7 @@
         <v>382</v>
       </c>
       <c r="C237" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D237" t="s">
         <v>258</v>
@@ -6205,7 +6205,7 @@
         <v>384</v>
       </c>
       <c r="C238" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D238" t="s">
         <v>258</v>
@@ -6233,7 +6233,7 @@
         <v>388</v>
       </c>
       <c r="C240" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D240" t="s">
         <v>258</v>
@@ -6325,10 +6325,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="B247" t="s">
         <v>714</v>
-      </c>
-      <c r="B247" t="s">
-        <v>715</v>
       </c>
       <c r="C247" t="s">
         <v>205</v>
@@ -6471,7 +6471,7 @@
         <v>275</v>
       </c>
       <c r="C257" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D257" t="s">
         <v>258</v>
@@ -6485,7 +6485,7 @@
         <v>180</v>
       </c>
       <c r="C258" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D258" t="s">
         <v>258</v>
@@ -6527,7 +6527,7 @@
         <v>188</v>
       </c>
       <c r="C261" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D261" t="s">
         <v>258</v>
@@ -6535,10 +6535,10 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="B262" t="s">
         <v>716</v>
-      </c>
-      <c r="B262" t="s">
-        <v>717</v>
       </c>
       <c r="C262" t="s">
         <v>205</v>
@@ -6555,7 +6555,7 @@
         <v>417</v>
       </c>
       <c r="C263" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D263" t="s">
         <v>258</v>
@@ -6611,7 +6611,7 @@
         <v>202</v>
       </c>
       <c r="C267" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D267" t="s">
         <v>258</v>
@@ -6717,7 +6717,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B275" t="s">
         <v>434</v>
@@ -6759,7 +6759,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B278" t="s">
         <v>438</v>
@@ -7269,7 +7269,7 @@
         <v>105</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D314" t="s">
         <v>2</v>
@@ -7283,7 +7283,7 @@
         <v>483</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D315" t="s">
         <v>2</v>
@@ -7291,10 +7291,10 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
+        <v>719</v>
+      </c>
+      <c r="B316" t="s">
         <v>720</v>
-      </c>
-      <c r="B316" t="s">
-        <v>721</v>
       </c>
       <c r="C316" t="s">
         <v>205</v>
@@ -7305,10 +7305,10 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
+        <v>721</v>
+      </c>
+      <c r="B317" t="s">
         <v>722</v>
-      </c>
-      <c r="B317" t="s">
-        <v>723</v>
       </c>
       <c r="C317" t="s">
         <v>205</v>
@@ -7325,7 +7325,7 @@
         <v>485</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D318" t="s">
         <v>2</v>
@@ -7353,7 +7353,7 @@
         <v>489</v>
       </c>
       <c r="C320" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D320" t="s">
         <v>2</v>
@@ -7403,10 +7403,10 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
+        <v>723</v>
+      </c>
+      <c r="B324" t="s">
         <v>724</v>
-      </c>
-      <c r="B324" t="s">
-        <v>725</v>
       </c>
       <c r="C324" t="s">
         <v>205</v>
@@ -7515,10 +7515,10 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A332" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B332" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C332" t="s">
         <v>7</v>
@@ -7633,7 +7633,7 @@
         <v>506</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D340" t="s">
         <v>2</v>
@@ -7784,7 +7784,7 @@
         <v>519</v>
       </c>
       <c r="B351" t="s">
-        <v>520</v>
+        <v>742</v>
       </c>
       <c r="C351" t="s">
         <v>16</v>
@@ -7795,10 +7795,10 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
+        <v>520</v>
+      </c>
+      <c r="B352" t="s">
         <v>521</v>
-      </c>
-      <c r="B352" t="s">
-        <v>522</v>
       </c>
       <c r="C352" t="s">
         <v>7</v>
@@ -7812,10 +7812,10 @@
         <v>177</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D353" t="s">
         <v>2</v>
@@ -7823,10 +7823,10 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
+        <v>523</v>
+      </c>
+      <c r="B354" t="s">
         <v>524</v>
-      </c>
-      <c r="B354" t="s">
-        <v>525</v>
       </c>
       <c r="C354" t="s">
         <v>205</v>
@@ -7851,13 +7851,13 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A356" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B356" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="B356" s="1" t="s">
-        <v>527</v>
-      </c>
       <c r="C356" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D356" t="s">
         <v>2</v>
@@ -7865,7 +7865,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B357" t="s">
         <v>516</v>
@@ -7879,10 +7879,10 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
+        <v>528</v>
+      </c>
+      <c r="B358" t="s">
         <v>529</v>
-      </c>
-      <c r="B358" t="s">
-        <v>530</v>
       </c>
       <c r="C358" t="s">
         <v>7</v>
@@ -7893,10 +7893,10 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
+        <v>530</v>
+      </c>
+      <c r="B359" t="s">
         <v>531</v>
-      </c>
-      <c r="B359" t="s">
-        <v>532</v>
       </c>
       <c r="C359" t="s">
         <v>7</v>
@@ -7921,10 +7921,10 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
+        <v>532</v>
+      </c>
+      <c r="B361" t="s">
         <v>533</v>
-      </c>
-      <c r="B361" t="s">
-        <v>534</v>
       </c>
       <c r="C361" t="s">
         <v>7</v>
@@ -7935,10 +7935,10 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
+        <v>534</v>
+      </c>
+      <c r="B362" t="s">
         <v>535</v>
-      </c>
-      <c r="B362" t="s">
-        <v>536</v>
       </c>
       <c r="C362" t="s">
         <v>7</v>
@@ -7949,10 +7949,10 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A363" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B363" t="s">
         <v>537</v>
-      </c>
-      <c r="B363" t="s">
-        <v>538</v>
       </c>
       <c r="C363" t="s">
         <v>7</v>
@@ -7963,10 +7963,10 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A364" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B364" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C364" t="s">
         <v>205</v>
@@ -7977,10 +7977,10 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A365" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B365" t="s">
         <v>541</v>
-      </c>
-      <c r="B365" t="s">
-        <v>542</v>
       </c>
       <c r="C365" t="s">
         <v>205</v>
@@ -7991,10 +7991,10 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B366" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C366" t="s">
         <v>205</v>
@@ -8005,10 +8005,10 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B367" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C367" t="s">
         <v>205</v>
@@ -8019,10 +8019,10 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B368" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C368" t="s">
         <v>205</v>
@@ -8033,10 +8033,10 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
+        <v>546</v>
+      </c>
+      <c r="B369" t="s">
         <v>547</v>
-      </c>
-      <c r="B369" t="s">
-        <v>548</v>
       </c>
       <c r="C369" t="s">
         <v>205</v>
@@ -8047,10 +8047,10 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B370" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C370" t="s">
         <v>205</v>
@@ -8061,10 +8061,10 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
+        <v>549</v>
+      </c>
+      <c r="B371" t="s">
         <v>550</v>
-      </c>
-      <c r="B371" t="s">
-        <v>551</v>
       </c>
       <c r="C371" t="s">
         <v>205</v>
@@ -8075,10 +8075,10 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
+        <v>551</v>
+      </c>
+      <c r="B372" t="s">
         <v>552</v>
-      </c>
-      <c r="B372" t="s">
-        <v>553</v>
       </c>
       <c r="C372" t="s">
         <v>205</v>
@@ -8089,10 +8089,10 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
+        <v>553</v>
+      </c>
+      <c r="B373" t="s">
         <v>554</v>
-      </c>
-      <c r="B373" t="s">
-        <v>555</v>
       </c>
       <c r="C373" t="s">
         <v>205</v>
@@ -8103,10 +8103,10 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
+        <v>555</v>
+      </c>
+      <c r="B374" t="s">
         <v>556</v>
-      </c>
-      <c r="B374" t="s">
-        <v>557</v>
       </c>
       <c r="C374" t="s">
         <v>205</v>
@@ -8117,10 +8117,10 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
+        <v>557</v>
+      </c>
+      <c r="B375" t="s">
         <v>558</v>
-      </c>
-      <c r="B375" t="s">
-        <v>559</v>
       </c>
       <c r="C375" t="s">
         <v>205</v>
@@ -8131,10 +8131,10 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
+        <v>559</v>
+      </c>
+      <c r="B376" t="s">
         <v>560</v>
-      </c>
-      <c r="B376" t="s">
-        <v>561</v>
       </c>
       <c r="C376" t="s">
         <v>205</v>
@@ -8145,10 +8145,10 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
+        <v>564</v>
+      </c>
+      <c r="B377" t="s">
         <v>565</v>
-      </c>
-      <c r="B377" t="s">
-        <v>566</v>
       </c>
       <c r="C377" t="s">
         <v>205</v>
@@ -8159,10 +8159,10 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
+        <v>566</v>
+      </c>
+      <c r="B378" t="s">
         <v>567</v>
-      </c>
-      <c r="B378" t="s">
-        <v>568</v>
       </c>
       <c r="C378" t="s">
         <v>205</v>
@@ -8173,10 +8173,10 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A379" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B379" t="s">
         <v>569</v>
-      </c>
-      <c r="B379" t="s">
-        <v>570</v>
       </c>
       <c r="C379" t="s">
         <v>205</v>
@@ -8187,10 +8187,10 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B380" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C380" t="s">
         <v>205</v>
@@ -8201,10 +8201,10 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
+        <v>727</v>
+      </c>
+      <c r="B381" t="s">
         <v>728</v>
-      </c>
-      <c r="B381" t="s">
-        <v>729</v>
       </c>
       <c r="C381" t="s">
         <v>205</v>
@@ -8215,10 +8215,10 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B382" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C382" t="s">
         <v>205</v>
@@ -8229,10 +8229,10 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
+        <v>570</v>
+      </c>
+      <c r="B383" t="s">
         <v>571</v>
-      </c>
-      <c r="B383" t="s">
-        <v>572</v>
       </c>
       <c r="C383" t="s">
         <v>205</v>
@@ -8243,10 +8243,10 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A384" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="B384" t="s">
         <v>573</v>
-      </c>
-      <c r="B384" t="s">
-        <v>574</v>
       </c>
       <c r="C384" t="s">
         <v>205</v>
@@ -8257,10 +8257,10 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A385" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B385" t="s">
         <v>732</v>
-      </c>
-      <c r="B385" t="s">
-        <v>733</v>
       </c>
       <c r="C385" t="s">
         <v>205</v>
@@ -8271,10 +8271,10 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A386" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B386" t="s">
         <v>575</v>
-      </c>
-      <c r="B386" t="s">
-        <v>576</v>
       </c>
       <c r="C386" t="s">
         <v>205</v>
@@ -8285,10 +8285,10 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B387" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C387" t="s">
         <v>205</v>
@@ -8299,10 +8299,10 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
+        <v>733</v>
+      </c>
+      <c r="B388" t="s">
         <v>734</v>
-      </c>
-      <c r="B388" t="s">
-        <v>735</v>
       </c>
       <c r="C388" t="s">
         <v>205</v>
@@ -8313,10 +8313,10 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
+        <v>577</v>
+      </c>
+      <c r="B389" t="s">
         <v>578</v>
-      </c>
-      <c r="B389" t="s">
-        <v>579</v>
       </c>
       <c r="C389" t="s">
         <v>205</v>
@@ -8327,10 +8327,10 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
+        <v>735</v>
+      </c>
+      <c r="B390" t="s">
         <v>736</v>
-      </c>
-      <c r="B390" t="s">
-        <v>737</v>
       </c>
       <c r="C390" t="s">
         <v>205</v>
@@ -8341,10 +8341,10 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A391" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="B391" t="s">
         <v>580</v>
-      </c>
-      <c r="B391" t="s">
-        <v>581</v>
       </c>
       <c r="C391" t="s">
         <v>205</v>
@@ -8355,10 +8355,10 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B392" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C392" t="s">
         <v>205</v>
@@ -8369,10 +8369,10 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B393" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C393" t="s">
         <v>205</v>
@@ -8383,10 +8383,10 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
+        <v>583</v>
+      </c>
+      <c r="B394" t="s">
         <v>584</v>
-      </c>
-      <c r="B394" t="s">
-        <v>585</v>
       </c>
       <c r="C394" t="s">
         <v>205</v>
@@ -8397,10 +8397,10 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
+        <v>585</v>
+      </c>
+      <c r="B395" t="s">
         <v>586</v>
-      </c>
-      <c r="B395" t="s">
-        <v>587</v>
       </c>
       <c r="C395" t="s">
         <v>205</v>
@@ -8411,10 +8411,10 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
+        <v>587</v>
+      </c>
+      <c r="B396" t="s">
         <v>588</v>
-      </c>
-      <c r="B396" t="s">
-        <v>589</v>
       </c>
       <c r="C396" t="s">
         <v>205</v>
@@ -8425,10 +8425,10 @@
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
+        <v>589</v>
+      </c>
+      <c r="B397" t="s">
         <v>590</v>
-      </c>
-      <c r="B397" t="s">
-        <v>591</v>
       </c>
       <c r="C397" t="s">
         <v>7</v>
@@ -8439,10 +8439,10 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A398" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="B398" t="s">
         <v>592</v>
-      </c>
-      <c r="B398" t="s">
-        <v>593</v>
       </c>
       <c r="C398" t="s">
         <v>7</v>
@@ -8453,10 +8453,10 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
+        <v>593</v>
+      </c>
+      <c r="B399" t="s">
         <v>594</v>
-      </c>
-      <c r="B399" t="s">
-        <v>595</v>
       </c>
       <c r="C399" t="s">
         <v>205</v>
@@ -8467,10 +8467,10 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B400" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C400" t="s">
         <v>205</v>
@@ -8481,13 +8481,13 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A401" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C401" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D401" t="s">
         <v>2</v>
@@ -8495,10 +8495,10 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
+        <v>596</v>
+      </c>
+      <c r="B402" t="s">
         <v>597</v>
-      </c>
-      <c r="B402" t="s">
-        <v>598</v>
       </c>
       <c r="C402" t="s">
         <v>205</v>
@@ -8509,10 +8509,10 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
+        <v>598</v>
+      </c>
+      <c r="B403" t="s">
         <v>599</v>
-      </c>
-      <c r="B403" t="s">
-        <v>600</v>
       </c>
       <c r="C403" t="s">
         <v>205</v>
@@ -8523,10 +8523,10 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A404" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B404" t="s">
         <v>601</v>
-      </c>
-      <c r="B404" t="s">
-        <v>602</v>
       </c>
       <c r="C404" t="s">
         <v>205</v>
@@ -8537,10 +8537,10 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A405" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="B405" s="2" t="s">
         <v>738</v>
-      </c>
-      <c r="B405" s="2" t="s">
-        <v>739</v>
       </c>
       <c r="C405" t="s">
         <v>7</v>
@@ -8565,10 +8565,10 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
+        <v>640</v>
+      </c>
+      <c r="B407" t="s">
         <v>641</v>
-      </c>
-      <c r="B407" t="s">
-        <v>642</v>
       </c>
       <c r="C407" t="s">
         <v>7</v>
@@ -8579,10 +8579,10 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
+        <v>642</v>
+      </c>
+      <c r="B408" t="s">
         <v>643</v>
-      </c>
-      <c r="B408" t="s">
-        <v>644</v>
       </c>
       <c r="C408" t="s">
         <v>7</v>
@@ -8607,7 +8607,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B410" t="s">
         <v>454</v>
@@ -8621,10 +8621,10 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
+        <v>645</v>
+      </c>
+      <c r="B411" t="s">
         <v>646</v>
-      </c>
-      <c r="B411" t="s">
-        <v>647</v>
       </c>
       <c r="C411" t="s">
         <v>7</v>
@@ -8666,7 +8666,7 @@
         <v>304</v>
       </c>
       <c r="B414" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C414" t="s">
         <v>7</v>
@@ -8677,10 +8677,10 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
+        <v>648</v>
+      </c>
+      <c r="B415" t="s">
         <v>649</v>
-      </c>
-      <c r="B415" t="s">
-        <v>650</v>
       </c>
       <c r="C415" t="s">
         <v>7</v>
@@ -8691,7 +8691,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B416" t="s">
         <v>34</v>
@@ -8705,10 +8705,10 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
+        <v>651</v>
+      </c>
+      <c r="B417" t="s">
         <v>652</v>
-      </c>
-      <c r="B417" t="s">
-        <v>653</v>
       </c>
       <c r="C417" t="s">
         <v>7</v>
@@ -8719,10 +8719,10 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
+        <v>653</v>
+      </c>
+      <c r="B418" t="s">
         <v>654</v>
-      </c>
-      <c r="B418" t="s">
-        <v>655</v>
       </c>
       <c r="C418" t="s">
         <v>7</v>
@@ -8733,10 +8733,10 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
+        <v>655</v>
+      </c>
+      <c r="B419" t="s">
         <v>656</v>
-      </c>
-      <c r="B419" t="s">
-        <v>657</v>
       </c>
       <c r="C419" t="s">
         <v>7</v>
@@ -8775,10 +8775,10 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
+        <v>657</v>
+      </c>
+      <c r="B422" t="s">
         <v>658</v>
-      </c>
-      <c r="B422" t="s">
-        <v>659</v>
       </c>
       <c r="C422" t="s">
         <v>7</v>
@@ -8789,10 +8789,10 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
+        <v>659</v>
+      </c>
+      <c r="B423" t="s">
         <v>660</v>
-      </c>
-      <c r="B423" t="s">
-        <v>661</v>
       </c>
       <c r="C423" t="s">
         <v>7</v>
@@ -8806,10 +8806,10 @@
         <v>336</v>
       </c>
       <c r="B424" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C424" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D424" t="s">
         <v>3</v>
@@ -8817,7 +8817,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B425" t="s">
         <v>106</v>
@@ -8845,10 +8845,10 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
+        <v>663</v>
+      </c>
+      <c r="B427" t="s">
         <v>664</v>
-      </c>
-      <c r="B427" t="s">
-        <v>665</v>
       </c>
       <c r="C427" t="s">
         <v>7</v>
@@ -8859,10 +8859,10 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
+        <v>665</v>
+      </c>
+      <c r="B428" t="s">
         <v>666</v>
-      </c>
-      <c r="B428" t="s">
-        <v>667</v>
       </c>
       <c r="C428" t="s">
         <v>7</v>
@@ -8873,10 +8873,10 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
+        <v>667</v>
+      </c>
+      <c r="B429" t="s">
         <v>668</v>
-      </c>
-      <c r="B429" t="s">
-        <v>669</v>
       </c>
       <c r="C429" t="s">
         <v>7</v>
@@ -8887,10 +8887,10 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
+        <v>669</v>
+      </c>
+      <c r="B430" t="s">
         <v>670</v>
-      </c>
-      <c r="B430" t="s">
-        <v>671</v>
       </c>
       <c r="C430" t="s">
         <v>7</v>
@@ -8918,10 +8918,10 @@
         <v>505</v>
       </c>
       <c r="B432" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C432" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D432" t="s">
         <v>3</v>
@@ -8929,10 +8929,10 @@
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
+        <v>672</v>
+      </c>
+      <c r="B433" t="s">
         <v>673</v>
-      </c>
-      <c r="B433" t="s">
-        <v>674</v>
       </c>
       <c r="C433" t="s">
         <v>7</v>
@@ -8943,10 +8943,10 @@
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
+        <v>674</v>
+      </c>
+      <c r="B434" t="s">
         <v>675</v>
-      </c>
-      <c r="B434" t="s">
-        <v>676</v>
       </c>
       <c r="C434" t="s">
         <v>7</v>
@@ -8957,10 +8957,10 @@
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
+        <v>676</v>
+      </c>
+      <c r="B435" t="s">
         <v>677</v>
-      </c>
-      <c r="B435" t="s">
-        <v>678</v>
       </c>
       <c r="C435" t="s">
         <v>7</v>
@@ -8971,10 +8971,10 @@
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
+        <v>678</v>
+      </c>
+      <c r="B436" t="s">
         <v>679</v>
-      </c>
-      <c r="B436" t="s">
-        <v>680</v>
       </c>
       <c r="C436" t="s">
         <v>7</v>
@@ -8985,10 +8985,10 @@
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
+        <v>680</v>
+      </c>
+      <c r="B437" t="s">
         <v>681</v>
-      </c>
-      <c r="B437" t="s">
-        <v>682</v>
       </c>
       <c r="C437" t="s">
         <v>7</v>
@@ -8999,10 +8999,10 @@
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
+        <v>682</v>
+      </c>
+      <c r="B438" t="s">
         <v>683</v>
-      </c>
-      <c r="B438" t="s">
-        <v>684</v>
       </c>
       <c r="C438" t="s">
         <v>7</v>
@@ -9013,10 +9013,10 @@
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
+        <v>684</v>
+      </c>
+      <c r="B439" t="s">
         <v>685</v>
-      </c>
-      <c r="B439" t="s">
-        <v>686</v>
       </c>
       <c r="C439" t="s">
         <v>7</v>
@@ -9041,10 +9041,10 @@
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
+        <v>686</v>
+      </c>
+      <c r="B441" t="s">
         <v>687</v>
-      </c>
-      <c r="B441" t="s">
-        <v>688</v>
       </c>
       <c r="C441" t="s">
         <v>7</v>
@@ -9055,10 +9055,10 @@
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
+        <v>688</v>
+      </c>
+      <c r="B442" t="s">
         <v>689</v>
-      </c>
-      <c r="B442" t="s">
-        <v>690</v>
       </c>
       <c r="C442" t="s">
         <v>7</v>
@@ -9069,10 +9069,10 @@
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
+        <v>740</v>
+      </c>
+      <c r="B443" t="s">
         <v>741</v>
-      </c>
-      <c r="B443" t="s">
-        <v>742</v>
       </c>
       <c r="C443" t="s">
         <v>205</v>
@@ -9083,10 +9083,10 @@
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B444" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C444" t="s">
         <v>205</v>
@@ -9097,10 +9097,10 @@
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
+        <v>604</v>
+      </c>
+      <c r="B445" t="s">
         <v>605</v>
-      </c>
-      <c r="B445" t="s">
-        <v>606</v>
       </c>
       <c r="C445" t="s">
         <v>205</v>
@@ -9111,10 +9111,10 @@
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
+        <v>606</v>
+      </c>
+      <c r="B446" t="s">
         <v>607</v>
-      </c>
-      <c r="B446" t="s">
-        <v>608</v>
       </c>
       <c r="C446" t="s">
         <v>205</v>
@@ -9125,10 +9125,10 @@
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
+        <v>608</v>
+      </c>
+      <c r="B447" t="s">
         <v>609</v>
-      </c>
-      <c r="B447" t="s">
-        <v>610</v>
       </c>
       <c r="C447" t="s">
         <v>205</v>
@@ -9139,10 +9139,10 @@
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
+        <v>610</v>
+      </c>
+      <c r="B448" t="s">
         <v>611</v>
-      </c>
-      <c r="B448" t="s">
-        <v>612</v>
       </c>
       <c r="C448" t="s">
         <v>205</v>
@@ -9153,10 +9153,10 @@
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
+        <v>612</v>
+      </c>
+      <c r="B449" t="s">
         <v>613</v>
-      </c>
-      <c r="B449" t="s">
-        <v>614</v>
       </c>
       <c r="C449" t="s">
         <v>205</v>
@@ -9167,10 +9167,10 @@
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
+        <v>614</v>
+      </c>
+      <c r="B450" t="s">
         <v>615</v>
-      </c>
-      <c r="B450" t="s">
-        <v>616</v>
       </c>
       <c r="C450" t="s">
         <v>205</v>
@@ -9181,10 +9181,10 @@
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
+        <v>616</v>
+      </c>
+      <c r="B451" t="s">
         <v>617</v>
-      </c>
-      <c r="B451" t="s">
-        <v>618</v>
       </c>
       <c r="C451" t="s">
         <v>205</v>
@@ -9195,10 +9195,10 @@
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
+        <v>618</v>
+      </c>
+      <c r="B452" t="s">
         <v>619</v>
-      </c>
-      <c r="B452" t="s">
-        <v>620</v>
       </c>
       <c r="C452" t="s">
         <v>205</v>
@@ -9209,10 +9209,10 @@
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B453" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C453" t="s">
         <v>205</v>
@@ -9223,10 +9223,10 @@
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B454" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C454" t="s">
         <v>205</v>
@@ -9237,10 +9237,10 @@
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
+        <v>621</v>
+      </c>
+      <c r="B455" t="s">
         <v>622</v>
-      </c>
-      <c r="B455" t="s">
-        <v>623</v>
       </c>
       <c r="C455" t="s">
         <v>16</v>
@@ -9251,7 +9251,7 @@
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B456" t="s">
         <v>80</v>
@@ -9265,7 +9265,7 @@
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B457" t="s">
         <v>441</v>
@@ -9279,7 +9279,7 @@
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B458" t="s">
         <v>441</v>
@@ -9293,7 +9293,7 @@
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B459" t="s">
         <v>441</v>
@@ -9307,7 +9307,7 @@
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B460" t="s">
         <v>441</v>
@@ -9321,7 +9321,7 @@
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B461" t="s">
         <v>441</v>
@@ -9335,7 +9335,7 @@
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B462" t="s">
         <v>442</v>
@@ -9349,7 +9349,7 @@
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B463" t="s">
         <v>442</v>
@@ -9363,7 +9363,7 @@
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B464" t="s">
         <v>442</v>
@@ -9377,7 +9377,7 @@
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B465" t="s">
         <v>442</v>
@@ -9391,7 +9391,7 @@
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B466" t="s">
         <v>442</v>
@@ -9405,7 +9405,7 @@
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B467" t="s">
         <v>442</v>
@@ -9419,7 +9419,7 @@
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B468" t="s">
         <v>441</v>
@@ -9433,10 +9433,10 @@
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
+        <v>633</v>
+      </c>
+      <c r="B469" t="s">
         <v>634</v>
-      </c>
-      <c r="B469" t="s">
-        <v>635</v>
       </c>
       <c r="C469" t="s">
         <v>205</v>
@@ -9447,10 +9447,10 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B470" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C470" t="s">
         <v>205</v>
@@ -9464,7 +9464,7 @@
         <v>206</v>
       </c>
       <c r="B471" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C471" t="s">
         <v>7</v>
@@ -9475,10 +9475,10 @@
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
+        <v>636</v>
+      </c>
+      <c r="B472" t="s">
         <v>637</v>
-      </c>
-      <c r="B472" t="s">
-        <v>638</v>
       </c>
       <c r="C472" t="s">
         <v>7</v>
@@ -9489,10 +9489,10 @@
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
+        <v>638</v>
+      </c>
+      <c r="B473" t="s">
         <v>639</v>
-      </c>
-      <c r="B473" t="s">
-        <v>640</v>
       </c>
       <c r="C473" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
In theory have redone 01.R with the new 2023 Shriver data, and also marking codes with  'sp.' as location-dependent. Cross-referenced native status with master species list.
</commit_message>
<xml_diff>
--- a/data/raw/from-Master_species-list-with-native-status_LO.xlsx
+++ b/data/raw/from-Master_species-list-with-native-status_LO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1704" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2DF33F8-985F-4C86-A728-A6032D4B33A3}"/>
+  <xr:revisionPtr revIDLastSave="1745" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39DA5971-B51A-440C-B254-9B2BCAE0B655}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,11 @@
     <author>tc={FAA363BE-12C3-417C-915B-65F45AE58638}</author>
     <author>tc={79B7D5D7-598C-49BB-930B-2C2F21AF0021}</author>
     <author>tc={94C28270-043D-4F55-BE47-C9283CD3AE92}</author>
+    <author>tc={EA93E8C1-C365-4377-AE48-8B53EA7FB281}</author>
+    <author>tc={991A2DBB-3974-43D5-9589-9BD261710577}</author>
+    <author>tc={2858018A-31FC-4B6C-B200-578BBBBF4F68}</author>
     <author>tc={7563C7EA-E009-4402-AFFE-132040552110}</author>
+    <author>tc={470F9A74-7F13-4208-98C9-6D0E64D6A936}</author>
   </authors>
   <commentList>
     <comment ref="C3" authorId="0" shapeId="0" xr:uid="{CA867E6F-1549-45FA-9B8F-05BBAD859D47}">
@@ -104,12 +108,44 @@
     USDA code is CHPO12</t>
       </text>
     </comment>
-    <comment ref="A268" authorId="7" shapeId="0" xr:uid="{7563C7EA-E009-4402-AFFE-132040552110}">
+    <comment ref="C246" authorId="7" shapeId="0" xr:uid="{EA93E8C1-C365-4377-AE48-8B53EA7FB281}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Marked as both Native &amp; Introduced on USDA Plants</t>
+      </text>
+    </comment>
+    <comment ref="C248" authorId="8" shapeId="0" xr:uid="{991A2DBB-3974-43D5-9589-9BD261710577}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Marked as both Native &amp; Introduced on USDA Plants</t>
+      </text>
+    </comment>
+    <comment ref="C254" authorId="9" shapeId="0" xr:uid="{2858018A-31FC-4B6C-B200-578BBBBF4F68}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Marked as both Native &amp; Introduced on USDA Plants</t>
+      </text>
+    </comment>
+    <comment ref="A268" authorId="10" shapeId="0" xr:uid="{7563C7EA-E009-4402-AFFE-132040552110}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     USDA code is MILI5</t>
+      </text>
+    </comment>
+    <comment ref="C354" authorId="11" shapeId="0" xr:uid="{470F9A74-7F13-4208-98C9-6D0E64D6A936}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Marked as both Native &amp; Introduced on USDA Plants</t>
       </text>
     </comment>
   </commentList>
@@ -2437,15 +2473,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2460,8 +2496,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7505700" y="381000"/>
-          <a:ext cx="4352925" cy="1590675"/>
+          <a:off x="11292840" y="377190"/>
+          <a:ext cx="4352925" cy="2366010"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2519,6 +2555,24 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t> are same ones from Master.xlsx (CodeOriginal). I have noted in a comment when the official USDA Plants code is different.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Native/Unknown assigned when the vast majority of that genus are native according to USDA Plants, especially in Arizona.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Unknown native status assigned to known species when USDA Plants lists them as both native and invasive in the Southwest.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -2855,8 +2909,20 @@
   <threadedComment ref="A221" dT="2022-11-21T22:35:26.96" personId="{F6D947F2-70EB-49FE-98C8-0B8FA94EE0D0}" id="{94C28270-043D-4F55-BE47-C9283CD3AE92}">
     <text>USDA code is CHPO12</text>
   </threadedComment>
+  <threadedComment ref="C246" dT="2023-09-19T18:01:11.68" personId="{96B0CADE-2D3B-403C-841B-213C5C52B49A}" id="{EA93E8C1-C365-4377-AE48-8B53EA7FB281}">
+    <text>Marked as both Native &amp; Introduced on USDA Plants</text>
+  </threadedComment>
+  <threadedComment ref="C248" dT="2023-09-19T18:01:11.68" personId="{96B0CADE-2D3B-403C-841B-213C5C52B49A}" id="{991A2DBB-3974-43D5-9589-9BD261710577}">
+    <text>Marked as both Native &amp; Introduced on USDA Plants</text>
+  </threadedComment>
+  <threadedComment ref="C254" dT="2023-09-19T18:01:11.68" personId="{96B0CADE-2D3B-403C-841B-213C5C52B49A}" id="{2858018A-31FC-4B6C-B200-578BBBBF4F68}">
+    <text>Marked as both Native &amp; Introduced on USDA Plants</text>
+  </threadedComment>
   <threadedComment ref="A268" dT="2022-11-21T22:58:57.50" personId="{F6D947F2-70EB-49FE-98C8-0B8FA94EE0D0}" id="{7563C7EA-E009-4402-AFFE-132040552110}">
     <text>USDA code is MILI5</text>
+  </threadedComment>
+  <threadedComment ref="C354" dT="2023-09-19T18:01:11.68" personId="{96B0CADE-2D3B-403C-841B-213C5C52B49A}" id="{470F9A74-7F13-4208-98C9-6D0E64D6A936}">
+    <text>Marked as both Native &amp; Introduced on USDA Plants</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2866,8 +2932,8 @@
   <dimension ref="A1:D473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A333" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B351" sqref="B351"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B274" sqref="B274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5869,7 +5935,7 @@
         <v>710</v>
       </c>
       <c r="C214" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D214" t="s">
         <v>258</v>
@@ -6331,7 +6397,7 @@
         <v>714</v>
       </c>
       <c r="C247" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D247" t="s">
         <v>258</v>
@@ -6695,7 +6761,7 @@
         <v>437</v>
       </c>
       <c r="C273" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D273" t="s">
         <v>258</v>
@@ -6709,7 +6775,7 @@
         <v>433</v>
       </c>
       <c r="C274" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D274" t="s">
         <v>258</v>
@@ -6737,7 +6803,7 @@
         <v>435</v>
       </c>
       <c r="C276" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D276" t="s">
         <v>258</v>
@@ -7255,7 +7321,7 @@
         <v>481</v>
       </c>
       <c r="C313" t="s">
-        <v>205</v>
+        <v>690</v>
       </c>
       <c r="D313" t="s">
         <v>2</v>
@@ -7297,7 +7363,7 @@
         <v>720</v>
       </c>
       <c r="C316" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D316" t="s">
         <v>2</v>
@@ -7311,7 +7377,7 @@
         <v>722</v>
       </c>
       <c r="C317" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D317" t="s">
         <v>2</v>
@@ -7395,7 +7461,7 @@
         <v>109</v>
       </c>
       <c r="C323" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D323" t="s">
         <v>2</v>
@@ -7409,7 +7475,7 @@
         <v>724</v>
       </c>
       <c r="C324" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D324" t="s">
         <v>2</v>
@@ -7549,7 +7615,7 @@
         <v>141</v>
       </c>
       <c r="C334" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D334" t="s">
         <v>2</v>
@@ -7745,7 +7811,7 @@
         <v>160</v>
       </c>
       <c r="C348" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D348" t="s">
         <v>2</v>
@@ -8025,7 +8091,7 @@
         <v>562</v>
       </c>
       <c r="C368" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D368" t="s">
         <v>2</v>
@@ -8053,7 +8119,7 @@
         <v>563</v>
       </c>
       <c r="C370" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D370" t="s">
         <v>2</v>
@@ -8067,7 +8133,7 @@
         <v>550</v>
       </c>
       <c r="C371" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D371" t="s">
         <v>2</v>
@@ -8123,7 +8189,7 @@
         <v>558</v>
       </c>
       <c r="C375" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D375" t="s">
         <v>2</v>
@@ -8137,7 +8203,7 @@
         <v>560</v>
       </c>
       <c r="C376" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D376" t="s">
         <v>2</v>
@@ -8165,7 +8231,7 @@
         <v>567</v>
       </c>
       <c r="C378" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D378" t="s">
         <v>2</v>
@@ -8403,7 +8469,7 @@
         <v>586</v>
       </c>
       <c r="C395" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D395" t="s">
         <v>2</v>
@@ -8417,7 +8483,7 @@
         <v>588</v>
       </c>
       <c r="C396" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D396" t="s">
         <v>2</v>
@@ -8473,7 +8539,7 @@
         <v>595</v>
       </c>
       <c r="C400" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D400" t="s">
         <v>2</v>
@@ -8515,7 +8581,7 @@
         <v>599</v>
       </c>
       <c r="C403" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D403" t="s">
         <v>2</v>
@@ -9103,7 +9169,7 @@
         <v>605</v>
       </c>
       <c r="C445" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D445" t="s">
         <v>3</v>
@@ -9131,7 +9197,7 @@
         <v>609</v>
       </c>
       <c r="C447" t="s">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="D447" t="s">
         <v>3</v>
@@ -9201,7 +9267,7 @@
         <v>619</v>
       </c>
       <c r="C452" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D452" t="s">
         <v>3</v>
@@ -9453,7 +9519,7 @@
         <v>632</v>
       </c>
       <c r="C470" t="s">
-        <v>205</v>
+        <v>7</v>
       </c>
       <c r="D470" t="s">
         <v>3</v>

</xml_diff>